<commit_message>
split into x and y input
</commit_message>
<xml_diff>
--- a/Data/US_veh.xlsx
+++ b/Data/US_veh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IsaacEvans\Documents\Uni\AI\EV_affect_on_emissions\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DDC1CAF1-13C2-4A69-9B5F-2E3BD3A8BC4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD325B6-F7E4-4DF9-8F34-89F6CF15CD34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -697,21 +697,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -719,6 +711,14 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -3143,7 +3143,7 @@
   <dimension ref="A1:AD67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:G24"/>
+      <selection activeCell="A12" sqref="A12:T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4111,52 +4111,52 @@
       <c r="AC11" s="32"/>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A12" s="71" t="s">
+      <c r="A12" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="72"/>
-      <c r="C12" s="72"/>
-      <c r="D12" s="72"/>
-      <c r="E12" s="72"/>
-      <c r="F12" s="72"/>
-      <c r="G12" s="72"/>
-      <c r="H12" s="72"/>
-      <c r="I12" s="72"/>
-      <c r="J12" s="72"/>
-      <c r="K12" s="72"/>
-      <c r="L12" s="72"/>
-      <c r="M12" s="72"/>
-      <c r="N12" s="72"/>
-      <c r="O12" s="72"/>
-      <c r="P12" s="72"/>
-      <c r="Q12" s="72"/>
-      <c r="R12" s="72"/>
-      <c r="S12" s="72"/>
-      <c r="T12" s="72"/>
+      <c r="B12" s="67"/>
+      <c r="C12" s="67"/>
+      <c r="D12" s="67"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="67"/>
+      <c r="H12" s="67"/>
+      <c r="I12" s="67"/>
+      <c r="J12" s="67"/>
+      <c r="K12" s="67"/>
+      <c r="L12" s="67"/>
+      <c r="M12" s="67"/>
+      <c r="N12" s="67"/>
+      <c r="O12" s="67"/>
+      <c r="P12" s="67"/>
+      <c r="Q12" s="67"/>
+      <c r="R12" s="67"/>
+      <c r="S12" s="67"/>
+      <c r="T12" s="67"/>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A13" s="73" t="s">
+      <c r="A13" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="73"/>
-      <c r="C13" s="73"/>
-      <c r="D13" s="73"/>
-      <c r="E13" s="73"/>
-      <c r="F13" s="73"/>
-      <c r="G13" s="73"/>
-      <c r="H13" s="73"/>
-      <c r="I13" s="73"/>
-      <c r="J13" s="73"/>
-      <c r="K13" s="73"/>
-      <c r="L13" s="73"/>
-      <c r="M13" s="73"/>
-      <c r="N13" s="73"/>
-      <c r="O13" s="73"/>
-      <c r="P13" s="73"/>
-      <c r="Q13" s="73"/>
-      <c r="R13" s="73"/>
-      <c r="S13" s="73"/>
-      <c r="T13" s="73"/>
+      <c r="B13" s="69"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="69"/>
+      <c r="E13" s="69"/>
+      <c r="F13" s="69"/>
+      <c r="G13" s="69"/>
+      <c r="H13" s="69"/>
+      <c r="I13" s="69"/>
+      <c r="J13" s="69"/>
+      <c r="K13" s="69"/>
+      <c r="L13" s="69"/>
+      <c r="M13" s="69"/>
+      <c r="N13" s="69"/>
+      <c r="O13" s="69"/>
+      <c r="P13" s="69"/>
+      <c r="Q13" s="69"/>
+      <c r="R13" s="69"/>
+      <c r="S13" s="69"/>
+      <c r="T13" s="69"/>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="44" t="s">
@@ -4183,61 +4183,61 @@
       <c r="T14" s="43"/>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A15" s="74" t="s">
+      <c r="A15" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="73"/>
-      <c r="C15" s="73"/>
-      <c r="D15" s="73"/>
-      <c r="E15" s="73"/>
-      <c r="F15" s="73"/>
-      <c r="G15" s="73"/>
-      <c r="H15" s="73"/>
-      <c r="I15" s="73"/>
-      <c r="J15" s="73"/>
-      <c r="K15" s="73"/>
-      <c r="L15" s="73"/>
-      <c r="M15" s="73"/>
-      <c r="N15" s="73"/>
-      <c r="O15" s="73"/>
-      <c r="P15" s="73"/>
-      <c r="Q15" s="73"/>
-      <c r="R15" s="73"/>
-      <c r="S15" s="73"/>
-      <c r="T15" s="73"/>
-      <c r="U15" s="73"/>
-      <c r="V15" s="73"/>
-      <c r="W15" s="73"/>
-      <c r="X15" s="73"/>
-      <c r="Y15" s="73"/>
-      <c r="Z15" s="73"/>
-      <c r="AA15" s="73"/>
-      <c r="AB15" s="73"/>
-      <c r="AC15" s="73"/>
+      <c r="B15" s="69"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="69"/>
+      <c r="G15" s="69"/>
+      <c r="H15" s="69"/>
+      <c r="I15" s="69"/>
+      <c r="J15" s="69"/>
+      <c r="K15" s="69"/>
+      <c r="L15" s="69"/>
+      <c r="M15" s="69"/>
+      <c r="N15" s="69"/>
+      <c r="O15" s="69"/>
+      <c r="P15" s="69"/>
+      <c r="Q15" s="69"/>
+      <c r="R15" s="69"/>
+      <c r="S15" s="69"/>
+      <c r="T15" s="69"/>
+      <c r="U15" s="69"/>
+      <c r="V15" s="69"/>
+      <c r="W15" s="69"/>
+      <c r="X15" s="69"/>
+      <c r="Y15" s="69"/>
+      <c r="Z15" s="69"/>
+      <c r="AA15" s="69"/>
+      <c r="AB15" s="69"/>
+      <c r="AC15" s="69"/>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A16" s="71" t="s">
+      <c r="A16" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="71"/>
-      <c r="C16" s="71"/>
-      <c r="D16" s="71"/>
-      <c r="E16" s="72"/>
-      <c r="F16" s="72"/>
-      <c r="G16" s="72"/>
-      <c r="H16" s="72"/>
-      <c r="I16" s="72"/>
-      <c r="J16" s="72"/>
-      <c r="K16" s="72"/>
-      <c r="L16" s="72"/>
-      <c r="M16" s="72"/>
-      <c r="N16" s="72"/>
-      <c r="O16" s="72"/>
-      <c r="P16" s="72"/>
-      <c r="Q16" s="72"/>
-      <c r="R16" s="72"/>
-      <c r="S16" s="72"/>
-      <c r="T16" s="72"/>
+      <c r="B16" s="66"/>
+      <c r="C16" s="66"/>
+      <c r="D16" s="66"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="67"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="67"/>
+      <c r="I16" s="67"/>
+      <c r="J16" s="67"/>
+      <c r="K16" s="67"/>
+      <c r="L16" s="67"/>
+      <c r="M16" s="67"/>
+      <c r="N16" s="67"/>
+      <c r="O16" s="67"/>
+      <c r="P16" s="67"/>
+      <c r="Q16" s="67"/>
+      <c r="R16" s="67"/>
+      <c r="S16" s="67"/>
+      <c r="T16" s="67"/>
     </row>
     <row r="17" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="68" t="s">
@@ -4312,15 +4312,15 @@
       <c r="T19" s="34"/>
     </row>
     <row r="20" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="69" t="s">
+      <c r="A20" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="69"/>
-      <c r="C20" s="69"/>
-      <c r="D20" s="69"/>
-      <c r="E20" s="69"/>
-      <c r="F20" s="69"/>
-      <c r="G20" s="69"/>
+      <c r="B20" s="73"/>
+      <c r="C20" s="73"/>
+      <c r="D20" s="73"/>
+      <c r="E20" s="73"/>
+      <c r="F20" s="73"/>
+      <c r="G20" s="73"/>
       <c r="H20" s="34"/>
       <c r="I20" s="34"/>
       <c r="J20" s="34"/>
@@ -4384,37 +4384,37 @@
       <c r="T22" s="34"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="70"/>
-      <c r="B23" s="66"/>
-      <c r="C23" s="66"/>
-      <c r="D23" s="66"/>
-      <c r="E23" s="66"/>
-      <c r="F23" s="66"/>
-      <c r="G23" s="66"/>
-      <c r="H23" s="66"/>
-      <c r="I23" s="66"/>
-      <c r="J23" s="66"/>
-      <c r="K23" s="66"/>
-      <c r="L23" s="66"/>
-      <c r="M23" s="66"/>
-      <c r="N23" s="66"/>
-      <c r="O23" s="66"/>
-      <c r="P23" s="66"/>
-      <c r="Q23" s="66"/>
-      <c r="R23" s="66"/>
-      <c r="S23" s="66"/>
-      <c r="T23" s="66"/>
+      <c r="A23" s="74"/>
+      <c r="B23" s="71"/>
+      <c r="C23" s="71"/>
+      <c r="D23" s="71"/>
+      <c r="E23" s="71"/>
+      <c r="F23" s="71"/>
+      <c r="G23" s="71"/>
+      <c r="H23" s="71"/>
+      <c r="I23" s="71"/>
+      <c r="J23" s="71"/>
+      <c r="K23" s="71"/>
+      <c r="L23" s="71"/>
+      <c r="M23" s="71"/>
+      <c r="N23" s="71"/>
+      <c r="O23" s="71"/>
+      <c r="P23" s="71"/>
+      <c r="Q23" s="71"/>
+      <c r="R23" s="71"/>
+      <c r="S23" s="71"/>
+      <c r="T23" s="71"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="66" t="s">
+      <c r="A24" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="66"/>
-      <c r="C24" s="66"/>
-      <c r="D24" s="66"/>
-      <c r="E24" s="66"/>
-      <c r="F24" s="66"/>
-      <c r="G24" s="66"/>
+      <c r="B24" s="71"/>
+      <c r="C24" s="71"/>
+      <c r="D24" s="71"/>
+      <c r="E24" s="71"/>
+      <c r="F24" s="71"/>
+      <c r="G24" s="71"/>
       <c r="H24" s="33"/>
       <c r="I24" s="33"/>
       <c r="J24" s="33"/>
@@ -4430,15 +4430,15 @@
       <c r="T24" s="33"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25" s="67" t="s">
+      <c r="A25" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="67"/>
-      <c r="C25" s="67"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="67"/>
-      <c r="F25" s="67"/>
-      <c r="G25" s="67"/>
+      <c r="B25" s="72"/>
+      <c r="C25" s="72"/>
+      <c r="D25" s="72"/>
+      <c r="E25" s="72"/>
+      <c r="F25" s="72"/>
+      <c r="G25" s="72"/>
       <c r="H25" s="33"/>
       <c r="I25" s="33"/>
       <c r="J25" s="33"/>
@@ -4459,11 +4459,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A16:T16"/>
-    <mergeCell ref="A12:T12"/>
-    <mergeCell ref="A17:G17"/>
-    <mergeCell ref="A13:T13"/>
-    <mergeCell ref="A15:AC15"/>
     <mergeCell ref="A24:G24"/>
     <mergeCell ref="A25:G25"/>
     <mergeCell ref="A18:G18"/>
@@ -4472,6 +4467,11 @@
     <mergeCell ref="A21:G21"/>
     <mergeCell ref="A23:T23"/>
     <mergeCell ref="A22:G22"/>
+    <mergeCell ref="A16:T16"/>
+    <mergeCell ref="A12:T12"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="A13:T13"/>
+    <mergeCell ref="A15:AC15"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>